<commit_message>
update jumps_battery summary_plots update plank summary_plots update isokinetic1rmtest_battery summary_plots
</commit_message>
<xml_diff>
--- a/src/labanalysis/testprotocols/normative_values.xlsx
+++ b/src/labanalysis/testprotocols/normative_values.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://technogymspa.sharepoint.com/sites/ScientificResearch/Shared Documents/t-lab/cesena_calcio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzoffoli\OneDrive - Technogym SPA\custom_app\labanalysis\src\labanalysis\testprotocols\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_9F1547B958AC403C5070FD602F37014B209CADBC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FE7EC71-EC65-448F-B43A-FCC7D95187A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7659C302-694D-4FE7-9ECB-E82DC1120D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9132" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CounterMovementJumpTest" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="22">
   <si>
     <t>Test</t>
   </si>
@@ -51,9 +51,6 @@
     <t>%</t>
   </si>
   <si>
-    <t>Efficiency</t>
-  </si>
-  <si>
     <t>Elevation</t>
   </si>
   <si>
@@ -94,15 +91,6 @@
   </si>
   <si>
     <t>LegPressREV</t>
-  </si>
-  <si>
-    <t>Side</t>
-  </si>
-  <si>
-    <t>Left</t>
-  </si>
-  <si>
-    <t>Right</t>
   </si>
 </sst>
 </file>
@@ -465,16 +453,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -505,13 +490,13 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>13.13357414404102</v>
       </c>
       <c r="F2">
-        <v>16.849004619454131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10.42215195061668</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -522,16 +507,16 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>93.364100153189668</v>
+        <v>39.028553819251421</v>
       </c>
       <c r="F3">
-        <v>3.9829414389394162</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5.7362121865701647</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -539,19 +524,19 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>39.028553819251421</v>
+        <v>2.6461569445884678</v>
       </c>
       <c r="F4">
-        <v>5.7362121865701647</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.2708224588218473</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -559,36 +544,16 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E5">
-        <v>2.6461569445884678</v>
+        <v>12.389385574927701</v>
       </c>
       <c r="F5">
-        <v>0.2708224588218473</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>50</v>
-      </c>
-      <c r="F6">
-        <v>15.319322808444641</v>
+        <v>8.8259765927145875</v>
       </c>
     </row>
   </sheetData>
@@ -600,13 +565,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,18 +586,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2">
         <v>42.520702826137907</v>
@@ -643,18 +606,18 @@
         <v>8.7031925974012108</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
       </c>
       <c r="E3">
         <v>2.9270018655638861</v>
@@ -674,9 +637,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,18 +656,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2">
         <v>55.981344266801031</v>
@@ -713,18 +676,18 @@
         <v>4.9613258155810982</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
       </c>
       <c r="E3">
         <v>2.4968424726216969</v>
@@ -740,18 +703,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -768,12 +726,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -782,90 +740,70 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>15.293450350057469</v>
       </c>
       <c r="F2">
-        <v>18.544242395797511</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10.21606206856281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>36.144752630096072</v>
+      </c>
+      <c r="F3">
+        <v>7.2163454617897349</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>2.7189206747848331</v>
+      </c>
+      <c r="F4">
+        <v>0.30110342647341087</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
-        <v>92.15119561685087</v>
-      </c>
-      <c r="F3">
-        <v>5.0199166047987456</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>36.144752630096072</v>
-      </c>
-      <c r="F4">
-        <v>7.2163454617897349</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
       <c r="E5">
-        <v>2.7189206747848331</v>
+        <v>16.889017892841899</v>
       </c>
       <c r="F5">
-        <v>0.30110342647341087</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>50.291845010355978</v>
-      </c>
-      <c r="F6">
-        <v>22.587136598730979</v>
+        <v>15.94143970007708</v>
       </c>
     </row>
   </sheetData>
@@ -879,20 +817,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -903,7 +841,7 @@
         <v>25.463651202102721</v>
       </c>
       <c r="D2">
-        <v>1.219762524809638</v>
+        <v>10.91633294725224</v>
       </c>
     </row>
   </sheetData>
@@ -913,390 +851,52 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>57.956642940865123</v>
       </c>
       <c r="D2">
-        <v>57.956642940865123</v>
-      </c>
-      <c r="E2">
         <v>19.040454597976758</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>178.97443861606899</v>
       </c>
       <c r="D3">
-        <v>178.97443861606899</v>
-      </c>
-      <c r="E3">
-        <v>18.134280494350229</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4">
-        <v>57.956642940865123</v>
-      </c>
-      <c r="E4">
-        <v>19.040454597976758</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5">
-        <v>178.97443861606899</v>
-      </c>
-      <c r="E5">
         <v>18.134280494350229</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bdbcbfc3-52d8-40bf-9172-d977a57f917a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1f57c247-f137-47d4-b913-b2892e2c419e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007C899C095B997346B9F68F789AA34C4D" ma:contentTypeVersion="15" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="f5f363e89cac64d63568ddbe47e9f8bf">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bdbcbfc3-52d8-40bf-9172-d977a57f917a" xmlns:ns3="1f57c247-f137-47d4-b913-b2892e2c419e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d09230a63ad1eb4b8c87adc615b7f464" ns2:_="" ns3:_="">
-    <xsd:import namespace="bdbcbfc3-52d8-40bf-9172-d977a57f917a"/>
-    <xsd:import namespace="1f57c247-f137-47d4-b913-b2892e2c419e"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bdbcbfc3-52d8-40bf-9172-d977a57f917a" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Tag immagine" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="815d4632-c721-4ad3-b6a3-a549a9cab835" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="21" nillable="true" ma:displayName="Location" ma:description="" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1f57c247-f137-47d4-b913-b2892e2c419e" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{a115337e-6b9f-41c3-8797-45b1556af357}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="1f57c247-f137-47d4-b913-b2892e2c419e">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Condiviso con" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Condiviso con dettagli" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo di contenuto"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titolo"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B83B066E-8614-4643-9483-73EA6F565766}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bdbcbfc3-52d8-40bf-9172-d977a57f917a"/>
-    <ds:schemaRef ds:uri="1f57c247-f137-47d4-b913-b2892e2c419e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2CD8727-F7CF-4EC2-AA23-6181B4036129}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C1FB37-932A-4EE9-8EFE-8C3F9D88154F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bdbcbfc3-52d8-40bf-9172-d977a57f917a"/>
-    <ds:schemaRef ds:uri="1f57c247-f137-47d4-b913-b2892e2c419e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>